<commit_message>
images nuevo intento 3
</commit_message>
<xml_diff>
--- a/.catalog/catalog.xlsx
+++ b/.catalog/catalog.xlsx
@@ -70,7 +70,10 @@
 Detalle: con marca y sin marca</t>
   </si>
   <si>
-    <t>nombreimagen.jpg</t>
+    <t>image1.jpg</t>
+  </si>
+  <si>
+    <t>imagen2.jpg</t>
   </si>
   <si>
     <t>001</t>
@@ -489,9 +492,6 @@
   </si>
   <si>
     <t>BLANCO</t>
-  </si>
-  <si>
-    <t>image1.jpg</t>
   </si>
   <si>
     <t>image2.jpg</t>
@@ -1096,7 +1096,7 @@
     <xdr:ext cx="1285875" cy="1619250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image19.jpg"/>
+        <xdr:cNvPr id="0" name="image18.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1124,7 +1124,7 @@
     <xdr:ext cx="1638300" cy="1609725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1152,7 +1152,7 @@
     <xdr:ext cx="1533525" cy="1666875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image5.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1208,7 +1208,7 @@
     <xdr:ext cx="1590675" cy="1895475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1236,7 +1236,7 @@
     <xdr:ext cx="1390650" cy="2028825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1320,7 +1320,7 @@
     <xdr:ext cx="1495425" cy="1666875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png"/>
+        <xdr:cNvPr id="0" name="image14.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1348,7 +1348,7 @@
     <xdr:ext cx="1562100" cy="1552575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image18.png"/>
+        <xdr:cNvPr id="0" name="image17.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1376,7 +1376,7 @@
     <xdr:ext cx="1533525" cy="1895475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1404,7 +1404,7 @@
     <xdr:ext cx="1457325" cy="1885950"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image4.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1432,7 +1432,7 @@
     <xdr:ext cx="1457325" cy="1847850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.jpg"/>
+        <xdr:cNvPr id="0" name="image9.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1460,7 +1460,7 @@
     <xdr:ext cx="933450" cy="1952625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.jpg"/>
+        <xdr:cNvPr id="0" name="image15.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1544,7 +1544,7 @@
     <xdr:ext cx="1314450" cy="1504950"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image23.jpg"/>
+        <xdr:cNvPr id="0" name="image11.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1572,7 +1572,7 @@
     <xdr:ext cx="1828800" cy="1285875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1600,7 +1600,7 @@
     <xdr:ext cx="1981200" cy="1485900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.jpg"/>
+        <xdr:cNvPr id="0" name="image12.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1628,7 +1628,7 @@
     <xdr:ext cx="2057400" cy="1104900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.jpg"/>
+        <xdr:cNvPr id="0" name="image16.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1656,7 +1656,7 @@
     <xdr:ext cx="2028825" cy="1390650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.jpg"/>
+        <xdr:cNvPr id="0" name="image16.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1684,7 +1684,7 @@
     <xdr:ext cx="1914525" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.jpg"/>
+        <xdr:cNvPr id="0" name="image10.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1712,7 +1712,7 @@
     <xdr:ext cx="1771650" cy="1381125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.jpg"/>
+        <xdr:cNvPr id="0" name="image10.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1740,7 +1740,7 @@
     <xdr:ext cx="2019300" cy="1400175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image24.png"/>
+        <xdr:cNvPr id="0" name="image19.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1768,7 +1768,7 @@
     <xdr:ext cx="990600" cy="1447800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image24.png"/>
+        <xdr:cNvPr id="0" name="image19.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1796,7 +1796,7 @@
     <xdr:ext cx="1752600" cy="1857375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg"/>
+        <xdr:cNvPr id="0" name="image22.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1824,7 +1824,7 @@
     <xdr:ext cx="1524000" cy="1905000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.jpg"/>
+        <xdr:cNvPr id="0" name="image8.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1852,7 +1852,7 @@
     <xdr:ext cx="1571625" cy="1733550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg"/>
+        <xdr:cNvPr id="0" name="image22.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1880,7 +1880,7 @@
     <xdr:ext cx="1885950" cy="1733550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg"/>
+        <xdr:cNvPr id="0" name="image22.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1908,7 +1908,7 @@
     <xdr:ext cx="1619250" cy="1076325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg"/>
+        <xdr:cNvPr id="0" name="image22.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1936,7 +1936,7 @@
     <xdr:ext cx="2152650" cy="1704975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg"/>
+        <xdr:cNvPr id="0" name="image22.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1964,7 +1964,7 @@
     <xdr:ext cx="1323975" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.jpg"/>
+        <xdr:cNvPr id="0" name="image8.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1992,7 +1992,7 @@
     <xdr:ext cx="1800225" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.jpg"/>
+        <xdr:cNvPr id="0" name="image8.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2020,7 +2020,7 @@
     <xdr:ext cx="1466850" cy="1247775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.jpg"/>
+        <xdr:cNvPr id="0" name="image8.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2048,7 +2048,7 @@
     <xdr:ext cx="1038225" cy="1447800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.jpg"/>
+        <xdr:cNvPr id="0" name="image23.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2076,7 +2076,7 @@
     <xdr:ext cx="1066800" cy="1476375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.jpg"/>
+        <xdr:cNvPr id="0" name="image23.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2104,7 +2104,7 @@
     <xdr:ext cx="2057400" cy="1066800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.jpg"/>
+        <xdr:cNvPr id="0" name="image23.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2132,7 +2132,7 @@
     <xdr:ext cx="1009650" cy="1428750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.jpg"/>
+        <xdr:cNvPr id="0" name="image23.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2160,7 +2160,7 @@
     <xdr:ext cx="1304925" cy="1704975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2188,7 +2188,7 @@
     <xdr:ext cx="1371600" cy="1704975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2216,7 +2216,7 @@
     <xdr:ext cx="1285875" cy="1828800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2244,7 +2244,7 @@
     <xdr:ext cx="1343025" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2272,7 +2272,7 @@
     <xdr:ext cx="1362075" cy="1762125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2300,7 +2300,7 @@
     <xdr:ext cx="1104900" cy="1771650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2328,7 +2328,7 @@
     <xdr:ext cx="1162050" cy="1733550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg"/>
+        <xdr:cNvPr id="0" name="image20.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2356,7 +2356,7 @@
     <xdr:ext cx="1876425" cy="1657350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image22.jpg"/>
+        <xdr:cNvPr id="0" name="image24.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2384,7 +2384,7 @@
     <xdr:ext cx="1362075" cy="1647825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image22.jpg"/>
+        <xdr:cNvPr id="0" name="image24.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2524,7 +2524,7 @@
     <xdr:ext cx="1466850" cy="1647825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image28.jpg"/>
+        <xdr:cNvPr id="0" name="image25.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2552,7 +2552,7 @@
     <xdr:ext cx="1581150" cy="1647825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image28.jpg"/>
+        <xdr:cNvPr id="0" name="image25.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2580,7 +2580,7 @@
     <xdr:ext cx="1400175" cy="1457325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image36.jpg"/>
+        <xdr:cNvPr id="0" name="image32.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2608,7 +2608,7 @@
     <xdr:ext cx="1543050" cy="1419225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image36.jpg"/>
+        <xdr:cNvPr id="0" name="image32.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2636,7 +2636,7 @@
     <xdr:ext cx="1476375" cy="1809750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image26.png"/>
+        <xdr:cNvPr id="0" name="image31.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2664,7 +2664,7 @@
     <xdr:ext cx="1495425" cy="1809750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image32.png"/>
+        <xdr:cNvPr id="0" name="image37.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2692,7 +2692,7 @@
     <xdr:ext cx="1447800" cy="1809750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image29.png"/>
+        <xdr:cNvPr id="0" name="image30.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2720,7 +2720,7 @@
     <xdr:ext cx="1466850" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image27.png"/>
+        <xdr:cNvPr id="0" name="image36.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2748,7 +2748,7 @@
     <xdr:ext cx="1485900" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image35.png"/>
+        <xdr:cNvPr id="0" name="image29.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2776,7 +2776,7 @@
     <xdr:ext cx="1438275" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image25.png"/>
+        <xdr:cNvPr id="0" name="image35.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2804,7 +2804,7 @@
     <xdr:ext cx="1419225" cy="1790700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image37.png"/>
+        <xdr:cNvPr id="0" name="image28.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2832,7 +2832,7 @@
     <xdr:ext cx="2514600" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2860,7 +2860,7 @@
     <xdr:ext cx="2514600" cy="1362075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image33.jpg"/>
+        <xdr:cNvPr id="0" name="image27.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2888,7 +2888,7 @@
     <xdr:ext cx="2276475" cy="1228725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image33.jpg"/>
+        <xdr:cNvPr id="0" name="image27.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2944,7 +2944,7 @@
     <xdr:ext cx="2514600" cy="933450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image31.jpg"/>
+        <xdr:cNvPr id="0" name="image26.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2972,7 +2972,7 @@
     <xdr:ext cx="2514600" cy="933450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image31.jpg"/>
+        <xdr:cNvPr id="0" name="image26.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3000,7 +3000,7 @@
     <xdr:ext cx="2514600" cy="933450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image31.jpg"/>
+        <xdr:cNvPr id="0" name="image26.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3028,7 +3028,7 @@
     <xdr:ext cx="2514600" cy="952500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.jpg"/>
+        <xdr:cNvPr id="0" name="image9.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3056,7 +3056,7 @@
     <xdr:ext cx="2514600" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.jpg"/>
+        <xdr:cNvPr id="0" name="image15.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3084,7 +3084,7 @@
     <xdr:ext cx="2276475" cy="828675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.jpg"/>
+        <xdr:cNvPr id="0" name="image15.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3112,7 +3112,7 @@
     <xdr:ext cx="2505075" cy="904875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.jpg"/>
+        <xdr:cNvPr id="0" name="image15.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3140,7 +3140,7 @@
     <xdr:ext cx="2514600" cy="1076325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image30.jpg"/>
+        <xdr:cNvPr id="0" name="image33.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3168,7 +3168,7 @@
     <xdr:ext cx="2514600" cy="1076325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image30.jpg"/>
+        <xdr:cNvPr id="0" name="image33.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3492,7 +3492,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="7">
         <v>0.0</v>
@@ -3501,16 +3501,16 @@
         <v>2000.0</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -3535,13 +3535,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -3556,16 +3556,16 @@
         <v>2000.0</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -3590,13 +3590,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -3611,16 +3611,16 @@
         <v>2000.0</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -3645,13 +3645,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -3666,16 +3666,16 @@
         <v>2000.0</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -3700,13 +3700,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -3721,16 +3721,16 @@
         <v>2000.0</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -3755,13 +3755,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3776,16 +3776,16 @@
         <v>2000.0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -3810,13 +3810,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -3831,16 +3831,16 @@
         <v>2000.0</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -3865,13 +3865,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -3886,16 +3886,16 @@
         <v>2000.0</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -3920,13 +3920,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -3941,16 +3941,16 @@
         <v>2000.0</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -3975,13 +3975,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -3996,16 +3996,16 @@
         <v>2000.0</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -4030,13 +4030,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -4051,16 +4051,16 @@
         <v>2000.0</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -4085,13 +4085,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -4106,16 +4106,16 @@
         <v>2000.0</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -4140,13 +4140,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -4161,16 +4161,16 @@
         <v>2000.0</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -4195,13 +4195,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4216,16 +4216,16 @@
         <v>2000.0</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -4250,13 +4250,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -4271,16 +4271,16 @@
         <v>2000.0</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -4305,13 +4305,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -4326,16 +4326,16 @@
         <v>2000.0</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
@@ -4360,13 +4360,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -4381,16 +4381,16 @@
         <v>2000.0</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N18" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
@@ -4415,13 +4415,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -4436,16 +4436,16 @@
         <v>2000.0</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O19" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -4470,13 +4470,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -4491,16 +4491,16 @@
         <v>2000.0</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N20" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -4525,13 +4525,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -4546,16 +4546,16 @@
         <v>2000.0</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N21" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -4580,13 +4580,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -4601,16 +4601,16 @@
         <v>2000.0</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N22" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -12844,7 +12844,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -12881,31 +12881,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -12930,20 +12930,20 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
@@ -12976,7 +12976,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D4" s="16">
         <v>2000.0</v>
@@ -12985,7 +12985,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>149</v>
+        <v>18</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>150</v>
@@ -13196,10 +13196,10 @@
     </row>
     <row r="9" ht="142.5" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>165</v>
@@ -13238,7 +13238,7 @@
     </row>
     <row r="10" ht="142.5" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>166</v>
@@ -13280,7 +13280,7 @@
     </row>
     <row r="11" ht="142.5" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>168</v>
@@ -13322,7 +13322,7 @@
     </row>
     <row r="12" ht="142.5" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>170</v>
@@ -13364,7 +13364,7 @@
     </row>
     <row r="13" ht="142.5" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>172</v>
@@ -13406,7 +13406,7 @@
     </row>
     <row r="14" ht="142.5" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>174</v>
@@ -13450,13 +13450,13 @@
     </row>
     <row r="15" ht="141.0" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D15" s="16">
         <v>2000.0</v>
@@ -13492,7 +13492,7 @@
     </row>
     <row r="16" ht="141.0" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>176</v>
@@ -13534,7 +13534,7 @@
     </row>
     <row r="17" ht="141.0" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>177</v>
@@ -13576,7 +13576,7 @@
     </row>
     <row r="18" ht="141.0" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>178</v>
@@ -13618,7 +13618,7 @@
     </row>
     <row r="19" ht="141.0" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>180</v>
@@ -13660,7 +13660,7 @@
     </row>
     <row r="20" ht="141.0" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>182</v>
@@ -13702,10 +13702,10 @@
     </row>
     <row r="21" ht="157.5" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>184</v>
@@ -13744,7 +13744,7 @@
     </row>
     <row r="22" ht="157.5" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>185</v>
@@ -13786,7 +13786,7 @@
     </row>
     <row r="23" ht="157.5" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>187</v>
@@ -13828,7 +13828,7 @@
     </row>
     <row r="24" ht="157.5" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>189</v>
@@ -13870,10 +13870,10 @@
     </row>
     <row r="25" ht="157.5" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>191</v>
@@ -13912,7 +13912,7 @@
     </row>
     <row r="26" ht="157.5" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>192</v>
@@ -13954,10 +13954,10 @@
     </row>
     <row r="27" ht="157.5" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>194</v>
@@ -13996,10 +13996,10 @@
     </row>
     <row r="28" ht="157.5" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>195</v>
@@ -14038,7 +14038,7 @@
     </row>
     <row r="29" ht="157.5" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>196</v>
@@ -14080,10 +14080,10 @@
     </row>
     <row r="30" ht="157.5" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>198</v>
@@ -14122,7 +14122,7 @@
     </row>
     <row r="31" ht="157.5" customHeight="1">
       <c r="A31" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>199</v>
@@ -14164,7 +14164,7 @@
     </row>
     <row r="32" ht="157.5" customHeight="1">
       <c r="A32" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>200</v>
@@ -14206,7 +14206,7 @@
     </row>
     <row r="33" ht="157.5" customHeight="1">
       <c r="A33" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>201</v>
@@ -14248,10 +14248,10 @@
     </row>
     <row r="34" ht="127.5" customHeight="1">
       <c r="A34" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>190</v>
@@ -14290,10 +14290,10 @@
     </row>
     <row r="35" ht="139.5" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="25" t="s">
         <v>202</v>
@@ -14332,7 +14332,7 @@
     </row>
     <row r="36" ht="139.5" customHeight="1">
       <c r="A36" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>203</v>
@@ -14374,7 +14374,7 @@
     </row>
     <row r="37" ht="139.5" customHeight="1">
       <c r="A37" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>205</v>
@@ -14416,7 +14416,7 @@
     </row>
     <row r="38" ht="141.75" customHeight="1">
       <c r="A38" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>207</v>
@@ -14458,7 +14458,7 @@
     </row>
     <row r="39" ht="141.75" customHeight="1">
       <c r="A39" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>209</v>
@@ -14500,7 +14500,7 @@
     </row>
     <row r="40" ht="125.25" customHeight="1">
       <c r="A40" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>211</v>
@@ -14542,10 +14542,10 @@
     </row>
     <row r="41" ht="121.5" customHeight="1">
       <c r="A41" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>212</v>
@@ -14584,7 +14584,7 @@
     </row>
     <row r="42" ht="121.5" customHeight="1">
       <c r="A42" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>213</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="43" ht="121.5" customHeight="1">
       <c r="A43" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>214</v>
@@ -14668,10 +14668,10 @@
     </row>
     <row r="44" ht="121.5" customHeight="1">
       <c r="A44" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="16">
@@ -14710,10 +14710,10 @@
     </row>
     <row r="45" ht="174.0" customHeight="1">
       <c r="A45" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>215</v>
@@ -14752,7 +14752,7 @@
     </row>
     <row r="46" ht="158.25" customHeight="1">
       <c r="A46" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>216</v>
@@ -14794,7 +14794,7 @@
     </row>
     <row r="47" ht="121.5" customHeight="1">
       <c r="A47" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>218</v>
@@ -14836,7 +14836,7 @@
     </row>
     <row r="48" ht="156.75" customHeight="1">
       <c r="A48" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>220</v>
@@ -14878,7 +14878,7 @@
     </row>
     <row r="49" ht="157.5" customHeight="1">
       <c r="A49" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>222</v>
@@ -14920,7 +14920,7 @@
     </row>
     <row r="50" ht="141.75" customHeight="1">
       <c r="A50" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>224</v>
@@ -14962,7 +14962,7 @@
     </row>
     <row r="51" ht="141.75" customHeight="1">
       <c r="A51" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>226</v>
@@ -15004,10 +15004,10 @@
     </row>
     <row r="52" ht="159.75" customHeight="1">
       <c r="A52" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>212</v>
@@ -15046,7 +15046,7 @@
     </row>
     <row r="53" ht="134.25" customHeight="1">
       <c r="A53" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>228</v>
@@ -15088,10 +15088,10 @@
     </row>
     <row r="54" ht="141.75" customHeight="1">
       <c r="A54" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>198</v>
@@ -15130,7 +15130,7 @@
     </row>
     <row r="55" ht="155.25" customHeight="1">
       <c r="A55" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>229</v>
@@ -15172,10 +15172,10 @@
     </row>
     <row r="56" ht="156.75" customHeight="1">
       <c r="A56" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>212</v>
@@ -15214,7 +15214,7 @@
     </row>
     <row r="57" ht="139.5" customHeight="1">
       <c r="A57" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>231</v>
@@ -15256,10 +15256,10 @@
     </row>
     <row r="58" ht="126.0" customHeight="1">
       <c r="A58" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>212</v>
@@ -15298,7 +15298,7 @@
     </row>
     <row r="59" ht="127.5" customHeight="1">
       <c r="A59" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>232</v>
@@ -15340,10 +15340,10 @@
     </row>
     <row r="60" ht="124.5" customHeight="1">
       <c r="A60" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="16">

</xml_diff>